<commit_message>
fix correlations of DFM, add toolbox VAR model, preprocess routines, add to do list
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\macrometrics-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C72105-21C5-4FD5-9974-4CFA11A49AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973785C6-9407-4CD2-97EE-843B7628CCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F32B473C-63B6-4416-A168-9B62820A9C8D}"/>
   </bookViews>
@@ -1387,7 +1387,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3">
-        <v>74.790000000000006</v>
+        <v>74.554266233300197</v>
       </c>
       <c r="K26" s="3">
         <v>100.55149</v>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="3">
-        <v>74.819999999999993</v>
+        <v>74.767995389553207</v>
       </c>
       <c r="K27" s="3">
         <v>100.67116</v>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="3">
-        <v>75.06</v>
+        <v>75.025232221685002</v>
       </c>
       <c r="K28" s="3">
         <v>99.063429999999997</v>
@@ -1515,7 +1515,7 @@
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="3">
-        <v>75.33</v>
+        <v>75.213535009398299</v>
       </c>
       <c r="K29" s="3">
         <v>97.402339999999995</v>
@@ -1557,7 +1557,7 @@
       </c>
       <c r="I30" s="2"/>
       <c r="J30" s="3">
-        <v>75.41</v>
+        <v>75.303250879404303</v>
       </c>
       <c r="K30" s="3">
         <v>95.909390000000002</v>
@@ -1599,7 +1599,7 @@
       </c>
       <c r="I31" s="2"/>
       <c r="J31" s="3">
-        <v>75.5</v>
+        <v>75.390579029903506</v>
       </c>
       <c r="K31" s="3">
         <v>94.072680000000005</v>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="3">
-        <v>75.760000000000005</v>
+        <v>75.623465698480999</v>
       </c>
       <c r="K32" s="3">
         <v>97.216489999999993</v>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="I33" s="2"/>
       <c r="J33" s="3">
-        <v>75.84</v>
+        <v>75.902295000944406</v>
       </c>
       <c r="K33" s="3">
         <v>96.426839999999999</v>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="3">
-        <v>75.900000000000006</v>
+        <v>76.136333784066807</v>
       </c>
       <c r="K34" s="3">
         <v>93.754400000000004</v>
@@ -1771,7 +1771,7 @@
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="3">
-        <v>76.23</v>
+        <v>76.312399536431698</v>
       </c>
       <c r="K35" s="3">
         <v>91.995930000000001</v>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="3">
-        <v>76.27</v>
+        <v>76.410272320537501</v>
       </c>
       <c r="K36" s="3">
         <v>90.562640000000002</v>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="3">
-        <v>76.430000000000007</v>
+        <v>76.564211100820899</v>
       </c>
       <c r="K37" s="3">
         <v>91.086910000000003</v>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="3">
-        <v>76.709999999999994</v>
+        <v>76.577407590622002</v>
       </c>
       <c r="K38" s="3">
         <v>94.023319999999998</v>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="3">
-        <v>76.400000000000006</v>
+        <v>76.497698553268194</v>
       </c>
       <c r="K39" s="3">
         <v>98.050139999999999</v>
@@ -1993,7 +1993,7 @@
       </c>
       <c r="I40" s="2"/>
       <c r="J40" s="3">
-        <v>76.63</v>
+        <v>76.709079908048693</v>
       </c>
       <c r="K40" s="3">
         <v>96.803529999999995</v>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="3">
-        <v>77.040000000000006</v>
+        <v>76.959299719528403</v>
       </c>
       <c r="K41" s="3">
         <v>97.472650000000002</v>
@@ -2083,7 +2083,7 @@
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="3">
-        <v>77.510000000000005</v>
+        <v>77.316228300148296</v>
       </c>
       <c r="K42" s="3">
         <v>97.011880000000005</v>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="3">
-        <v>77.87</v>
+        <v>77.666323420438204</v>
       </c>
       <c r="K43" s="3">
         <v>94.778130000000004</v>
@@ -2173,7 +2173,7 @@
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="3">
-        <v>77.989999999999995</v>
+        <v>77.798407598674203</v>
       </c>
       <c r="K44" s="3">
         <v>93.315899999999999</v>
@@ -2217,7 +2217,7 @@
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="3">
-        <v>77.81</v>
+        <v>77.847499066825193</v>
       </c>
       <c r="K45" s="3">
         <v>94.413610000000006</v>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="3">
-        <v>77.75</v>
+        <v>77.934802384068107</v>
       </c>
       <c r="K46" s="3">
         <v>97.57835</v>
@@ -2307,7 +2307,7 @@
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="3">
-        <v>77.959999999999994</v>
+        <v>78.025338434638698</v>
       </c>
       <c r="K47" s="3">
         <v>98.434119999999993</v>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="I48" s="2"/>
       <c r="J48" s="3">
-        <v>78.03</v>
+        <v>78.134095683090607</v>
       </c>
       <c r="K48" s="3">
         <v>98.218739999999997</v>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="I49" s="2"/>
       <c r="J49" s="3">
-        <v>77.98</v>
+        <v>78.151146770152096</v>
       </c>
       <c r="K49" s="3">
         <v>96.291610000000006</v>
@@ -2441,7 +2441,7 @@
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="3">
-        <v>78.319999999999993</v>
+        <v>78.261908745619095</v>
       </c>
       <c r="K50" s="3">
         <v>96.39564</v>
@@ -2487,7 +2487,7 @@
         <v>63.1</v>
       </c>
       <c r="J51" s="3">
-        <v>78.42</v>
+        <v>78.605535113098298</v>
       </c>
       <c r="K51" s="3">
         <v>96.39967</v>
@@ -2533,7 +2533,7 @@
         <v>64.400000000000006</v>
       </c>
       <c r="J52" s="3">
-        <v>78.55</v>
+        <v>78.686699838984694</v>
       </c>
       <c r="K52" s="3">
         <v>95.214740000000006</v>
@@ -2581,7 +2581,7 @@
         <v>66</v>
       </c>
       <c r="J53" s="3">
-        <v>78.989999999999995</v>
+        <v>78.803611906834803</v>
       </c>
       <c r="K53" s="3">
         <v>95.388379999999998</v>
@@ -2627,7 +2627,7 @@
         <v>64.7</v>
       </c>
       <c r="J54" s="3">
-        <v>79.349999999999994</v>
+        <v>79.190800616589598</v>
       </c>
       <c r="K54" s="3">
         <v>95.747219999999999</v>
@@ -2673,7 +2673,7 @@
         <v>66.3</v>
       </c>
       <c r="J55" s="3">
-        <v>79.489999999999995</v>
+        <v>79.242991912112203</v>
       </c>
       <c r="K55" s="3">
         <v>97.946669999999997</v>
@@ -2721,7 +2721,7 @@
         <v>66.599999999999994</v>
       </c>
       <c r="J56" s="3">
-        <v>79.459999999999994</v>
+        <v>79.261397828094601</v>
       </c>
       <c r="K56" s="3">
         <v>100.93223</v>
@@ -2767,7 +2767,7 @@
         <v>65.5</v>
       </c>
       <c r="J57" s="3">
-        <v>79.38</v>
+        <v>79.430554225519103</v>
       </c>
       <c r="K57" s="3">
         <v>103.07474999999999</v>
@@ -2813,7 +2813,7 @@
         <v>66.3</v>
       </c>
       <c r="J58" s="3">
-        <v>79.430000000000007</v>
+        <v>79.588301208133103</v>
       </c>
       <c r="K58" s="3">
         <v>102.50279</v>
@@ -2861,7 +2861,7 @@
         <v>65.900000000000006</v>
       </c>
       <c r="J59" s="3">
-        <v>79.63</v>
+        <v>79.684881421672003</v>
       </c>
       <c r="K59" s="3">
         <v>102.59659000000001</v>
@@ -2907,7 +2907,7 @@
         <v>66.900000000000006</v>
       </c>
       <c r="J60" s="3">
-        <v>79.819999999999993</v>
+        <v>79.881432755440798</v>
       </c>
       <c r="K60" s="3">
         <v>103.1541</v>
@@ -2953,7 +2953,7 @@
         <v>67.5</v>
       </c>
       <c r="J61" s="3">
-        <v>79.760000000000005</v>
+        <v>79.935743471737197</v>
       </c>
       <c r="K61" s="3">
         <v>103.81973000000001</v>
@@ -3001,7 +3001,7 @@
         <v>66.400000000000006</v>
       </c>
       <c r="J62" s="3">
-        <v>80.14</v>
+        <v>80.111211194700999</v>
       </c>
       <c r="K62" s="3">
         <v>104.61205</v>
@@ -3047,7 +3047,7 @@
         <v>67.099999999999994</v>
       </c>
       <c r="J63" s="3">
-        <v>80.11</v>
+        <v>80.3663100626447</v>
       </c>
       <c r="K63" s="3">
         <v>107.77302</v>
@@ -3093,7 +3093,7 @@
         <v>66.099999999999994</v>
       </c>
       <c r="J64" s="3">
-        <v>80.430000000000007</v>
+        <v>80.612238962174899</v>
       </c>
       <c r="K64" s="3">
         <v>108.93934</v>
@@ -3141,7 +3141,7 @@
         <v>64.7</v>
       </c>
       <c r="J65" s="3">
-        <v>80.89</v>
+        <v>80.798082032896502</v>
       </c>
       <c r="K65" s="3">
         <v>109.7109</v>
@@ -3187,7 +3187,7 @@
         <v>64.5</v>
       </c>
       <c r="J66" s="3">
-        <v>81.02</v>
+        <v>80.724018080050797</v>
       </c>
       <c r="K66" s="3">
         <v>109.77845000000001</v>
@@ -3233,7 +3233,7 @@
         <v>64.5</v>
       </c>
       <c r="J67" s="3">
-        <v>80.97</v>
+        <v>80.701894030741101</v>
       </c>
       <c r="K67" s="3">
         <v>113.62797999999999</v>
@@ -3281,7 +3281,7 @@
         <v>65.3</v>
       </c>
       <c r="J68" s="3">
-        <v>81.069999999999993</v>
+        <v>80.865073904476304</v>
       </c>
       <c r="K68" s="3">
         <v>113.75633000000001</v>
@@ -3327,7 +3327,7 @@
         <v>65.8</v>
       </c>
       <c r="J69" s="3">
-        <v>80.95</v>
+        <v>81.009450775838701</v>
       </c>
       <c r="K69" s="3">
         <v>112.33331</v>
@@ -3373,7 +3373,7 @@
         <v>66.099999999999994</v>
       </c>
       <c r="J70" s="3">
-        <v>81.069999999999993</v>
+        <v>81.197973263599593</v>
       </c>
       <c r="K70" s="3">
         <v>111.03588999999999</v>
@@ -3421,7 +3421,7 @@
         <v>66.5</v>
       </c>
       <c r="J71" s="3">
-        <v>81.36</v>
+        <v>81.394330946088303</v>
       </c>
       <c r="K71" s="3">
         <v>111.03694</v>
@@ -3467,7 +3467,7 @@
         <v>68.2</v>
       </c>
       <c r="J72" s="3">
-        <v>81.48</v>
+        <v>81.493325874176406</v>
       </c>
       <c r="K72" s="3">
         <v>113.03813</v>
@@ -3513,7 +3513,7 @@
         <v>67.5</v>
       </c>
       <c r="J73" s="3">
-        <v>81.510000000000005</v>
+        <v>81.664325500189804</v>
       </c>
       <c r="K73" s="3">
         <v>112.86304</v>
@@ -3561,7 +3561,7 @@
         <v>69.8</v>
       </c>
       <c r="J74" s="3">
-        <v>81.760000000000005</v>
+        <v>81.740338858978205</v>
       </c>
       <c r="K74" s="3">
         <v>115.96616</v>
@@ -3607,7 +3607,7 @@
         <v>69.2</v>
       </c>
       <c r="J75" s="3">
-        <v>81.58</v>
+        <v>81.934317415937301</v>
       </c>
       <c r="K75" s="3">
         <v>116.97895</v>
@@ -3653,7 +3653,7 @@
         <v>70.3</v>
       </c>
       <c r="J76" s="3">
-        <v>81.77</v>
+        <v>82.036440245415605</v>
       </c>
       <c r="K76" s="3">
         <v>116.23302</v>
@@ -3701,7 +3701,7 @@
         <v>70.400000000000006</v>
       </c>
       <c r="J77" s="3">
-        <v>82.29</v>
+        <v>82.234535106151597</v>
       </c>
       <c r="K77" s="3">
         <v>114.21006</v>
@@ -3747,7 +3747,7 @@
         <v>72.3</v>
       </c>
       <c r="J78" s="3">
-        <v>82.71</v>
+        <v>82.400173229801496</v>
       </c>
       <c r="K78" s="3">
         <v>112.58975</v>
@@ -3793,7 +3793,7 @@
         <v>72.8</v>
       </c>
       <c r="J79" s="3">
-        <v>82.98</v>
+        <v>82.674831369670798</v>
       </c>
       <c r="K79" s="3">
         <v>113.97366</v>
@@ -3841,7 +3841,7 @@
         <v>71.5</v>
       </c>
       <c r="J80" s="3">
-        <v>83.02</v>
+        <v>82.780515589659402</v>
       </c>
       <c r="K80" s="3">
         <v>113.82747999999999</v>
@@ -3887,7 +3887,7 @@
         <v>73.7</v>
       </c>
       <c r="J81" s="3">
-        <v>82.85</v>
+        <v>82.895010584527995</v>
       </c>
       <c r="K81" s="3">
         <v>113.99785</v>
@@ -3933,7 +3933,7 @@
         <v>70.3</v>
       </c>
       <c r="J82" s="3">
-        <v>83.01</v>
+        <v>83.101076073753106</v>
       </c>
       <c r="K82" s="3">
         <v>113.57717</v>
@@ -3981,7 +3981,7 @@
         <v>70.8</v>
       </c>
       <c r="J83" s="3">
-        <v>83.11</v>
+        <v>83.116961739774794</v>
       </c>
       <c r="K83" s="3">
         <v>114.23612</v>
@@ -4027,7 +4027,7 @@
         <v>73.5</v>
       </c>
       <c r="J84" s="3">
-        <v>83.43</v>
+        <v>83.393699999788694</v>
       </c>
       <c r="K84" s="3">
         <v>115.22723999999999</v>
@@ -4073,7 +4073,7 @@
         <v>72.3</v>
       </c>
       <c r="J85" s="3">
-        <v>83.37</v>
+        <v>83.498855908312393</v>
       </c>
       <c r="K85" s="3">
         <v>116.50005</v>
@@ -4121,7 +4121,7 @@
         <v>71.599999999999994</v>
       </c>
       <c r="J86" s="3">
-        <v>83.68</v>
+        <v>83.653809481250605</v>
       </c>
       <c r="K86" s="3">
         <v>117.36257000000001</v>
@@ -4167,7 +4167,7 @@
         <v>73.7</v>
       </c>
       <c r="J87" s="3">
-        <v>83.17</v>
+        <v>83.613500830505998</v>
       </c>
       <c r="K87" s="3">
         <v>116.29913000000001</v>
@@ -4213,7 +4213,7 @@
         <v>72.5</v>
       </c>
       <c r="J88" s="3">
-        <v>83.47</v>
+        <v>83.814180194825397</v>
       </c>
       <c r="K88" s="3">
         <v>114.37607</v>
@@ -4261,7 +4261,7 @@
         <v>73.400000000000006</v>
       </c>
       <c r="J89" s="3">
-        <v>84.09</v>
+        <v>83.969614904840199</v>
       </c>
       <c r="K89" s="3">
         <v>115.39357</v>
@@ -4307,7 +4307,7 @@
         <v>74.599999999999994</v>
       </c>
       <c r="J90" s="3">
-        <v>84.45</v>
+        <v>84.241170895942304</v>
       </c>
       <c r="K90" s="3">
         <v>114.59457999999999</v>
@@ -4353,7 +4353,7 @@
         <v>75.3</v>
       </c>
       <c r="J91" s="3">
-        <v>84.63</v>
+        <v>84.301237222672</v>
       </c>
       <c r="K91" s="3">
         <v>113.05583</v>
@@ -4401,7 +4401,7 @@
         <v>75.7</v>
       </c>
       <c r="J92" s="3">
-        <v>84.72</v>
+        <v>84.455302352789104</v>
       </c>
       <c r="K92" s="3">
         <v>109.95851</v>
@@ -4447,7 +4447,7 @@
         <v>77.599999999999994</v>
       </c>
       <c r="J93" s="3">
-        <v>84.63</v>
+        <v>84.664604281445605</v>
       </c>
       <c r="K93" s="3">
         <v>110.37392</v>
@@ -4493,7 +4493,7 @@
         <v>77.5</v>
       </c>
       <c r="J94" s="3">
-        <v>84.83</v>
+        <v>84.902931256022896</v>
       </c>
       <c r="K94" s="3">
         <v>110.6896</v>
@@ -4541,7 +4541,7 @@
         <v>78.599999999999994</v>
       </c>
       <c r="J95" s="3">
-        <v>85.27</v>
+        <v>85.259599708575294</v>
       </c>
       <c r="K95" s="3">
         <v>110.12461</v>
@@ -4587,7 +4587,7 @@
         <v>78.099999999999994</v>
       </c>
       <c r="J96" s="3">
-        <v>85.49</v>
+        <v>85.433991419797493</v>
       </c>
       <c r="K96" s="3">
         <v>109.42718000000001</v>
@@ -4633,7 +4633,7 @@
         <v>78.5</v>
       </c>
       <c r="J97" s="3">
-        <v>85.31</v>
+        <v>85.420766683152493</v>
       </c>
       <c r="K97" s="3">
         <v>108.38326000000001</v>
@@ -4681,7 +4681,7 @@
         <v>80</v>
       </c>
       <c r="J98" s="3">
-        <v>85.59</v>
+        <v>85.559659546838404</v>
       </c>
       <c r="K98" s="3">
         <v>108.38442999999999</v>
@@ -4727,7 +4727,7 @@
         <v>79.099999999999994</v>
       </c>
       <c r="J99" s="3">
-        <v>85.22</v>
+        <v>85.7267407911541</v>
       </c>
       <c r="K99" s="3">
         <v>109.62302</v>
@@ -4773,7 +4773,7 @@
         <v>80.5</v>
       </c>
       <c r="J100" s="3">
-        <v>85.46</v>
+        <v>85.8564541620581</v>
       </c>
       <c r="K100" s="3">
         <v>107.67639</v>
@@ -4821,7 +4821,7 @@
         <v>79.900000000000006</v>
       </c>
       <c r="J101" s="3">
-        <v>85.95</v>
+        <v>85.950953750299206</v>
       </c>
       <c r="K101" s="3">
         <v>108.74585</v>
@@ -4867,7 +4867,7 @@
         <v>82.8</v>
       </c>
       <c r="J102" s="3">
-        <v>86.52</v>
+        <v>86.183988466885793</v>
       </c>
       <c r="K102" s="3">
         <v>110.13203</v>
@@ -4913,7 +4913,7 @@
         <v>81.2</v>
       </c>
       <c r="J103" s="3">
-        <v>86.77</v>
+        <v>86.401446806872201</v>
       </c>
       <c r="K103" s="3">
         <v>111.79403000000001</v>
@@ -4961,7 +4961,7 @@
         <v>81.7</v>
       </c>
       <c r="J104" s="3">
-        <v>86.83</v>
+        <v>86.515289308115399</v>
       </c>
       <c r="K104" s="3">
         <v>112.20968000000001</v>
@@ -5007,7 +5007,7 @@
         <v>81.5</v>
       </c>
       <c r="J105" s="3">
-        <v>86.72</v>
+        <v>86.736426887917901</v>
       </c>
       <c r="K105" s="3">
         <v>112.11649</v>
@@ -5053,7 +5053,7 @@
         <v>82.2</v>
       </c>
       <c r="J106" s="3">
-        <v>86.8</v>
+        <v>86.872485913381894</v>
       </c>
       <c r="K106" s="3">
         <v>111.70493999999999</v>
@@ -5101,7 +5101,7 @@
         <v>86.2</v>
       </c>
       <c r="J107" s="3">
-        <v>86.81</v>
+        <v>86.815636447623206</v>
       </c>
       <c r="K107" s="3">
         <v>111.47242</v>
@@ -5147,7 +5147,7 @@
         <v>85.8</v>
       </c>
       <c r="J108" s="3">
-        <v>86.87</v>
+        <v>86.8331874620701</v>
       </c>
       <c r="K108" s="3">
         <v>110.69257</v>
@@ -5193,7 +5193,7 @@
         <v>86.9</v>
       </c>
       <c r="J109" s="3">
-        <v>86.91</v>
+        <v>87.008398764096</v>
       </c>
       <c r="K109" s="3">
         <v>111.51873000000001</v>
@@ -5241,7 +5241,7 @@
         <v>89.4</v>
       </c>
       <c r="J110" s="3">
-        <v>87.24</v>
+        <v>87.209500305259496</v>
       </c>
       <c r="K110" s="3">
         <v>112.58881</v>
@@ -5287,7 +5287,7 @@
         <v>86.2</v>
       </c>
       <c r="J111" s="3">
-        <v>86.81</v>
+        <v>87.367384069520199</v>
       </c>
       <c r="K111" s="3">
         <v>111.86772000000001</v>
@@ -5335,7 +5335,7 @@
         <v>86.3</v>
       </c>
       <c r="J112" s="3">
-        <v>87.06</v>
+        <v>87.493450328977602</v>
       </c>
       <c r="K112" s="3">
         <v>111.63847</v>
@@ -5385,7 +5385,7 @@
         <v>86.1</v>
       </c>
       <c r="J113" s="3">
-        <v>87.64</v>
+        <v>87.627920099077699</v>
       </c>
       <c r="K113" s="3">
         <v>112.66314</v>
@@ -5433,7 +5433,7 @@
         <v>86.4</v>
       </c>
       <c r="J114" s="3">
-        <v>88.2</v>
+        <v>87.854494114763298</v>
       </c>
       <c r="K114" s="3">
         <v>113.36846</v>
@@ -5481,7 +5481,7 @@
         <v>85.9</v>
       </c>
       <c r="J115" s="3">
-        <v>88.41</v>
+        <v>88.0190289540284</v>
       </c>
       <c r="K115" s="3">
         <v>113.3203</v>
@@ -5531,7 +5531,7 @@
         <v>87.7</v>
       </c>
       <c r="J116" s="3">
-        <v>88.49</v>
+        <v>88.136689713570206</v>
       </c>
       <c r="K116" s="3">
         <v>112.37433</v>
@@ -5579,7 +5579,7 @@
         <v>87</v>
       </c>
       <c r="J117" s="3">
-        <v>88.28</v>
+        <v>88.307142674034395</v>
       </c>
       <c r="K117" s="3">
         <v>112.72834</v>
@@ -5627,7 +5627,7 @@
         <v>90.1</v>
       </c>
       <c r="J118" s="3">
-        <v>88.35</v>
+        <v>88.446694373821003</v>
       </c>
       <c r="K118" s="3">
         <v>112.46825</v>
@@ -5677,7 +5677,7 @@
         <v>90.8</v>
       </c>
       <c r="J119" s="3">
-        <v>88.69</v>
+        <v>88.712509691665801</v>
       </c>
       <c r="K119" s="3">
         <v>113.33759000000001</v>
@@ -5725,7 +5725,7 @@
         <v>90.3</v>
       </c>
       <c r="J120" s="3">
-        <v>89.13</v>
+        <v>89.095480913114898</v>
       </c>
       <c r="K120" s="3">
         <v>114.15591000000001</v>
@@ -5773,7 +5773,7 @@
         <v>89.7</v>
       </c>
       <c r="J121" s="3">
-        <v>89.61</v>
+        <v>89.692359281368297</v>
       </c>
       <c r="K121" s="3">
         <v>115.75445000000001</v>
@@ -5823,7 +5823,7 @@
         <v>89.4</v>
       </c>
       <c r="J122" s="3">
-        <v>89.97</v>
+        <v>89.943155942863299</v>
       </c>
       <c r="K122" s="3">
         <v>115.66361000000001</v>
@@ -5871,7 +5871,7 @@
         <v>93</v>
       </c>
       <c r="J123" s="3">
-        <v>89.65</v>
+        <v>90.282640681077297</v>
       </c>
       <c r="K123" s="3">
         <v>116.51299</v>
@@ -5919,7 +5919,7 @@
         <v>91.9</v>
       </c>
       <c r="J124" s="3">
-        <v>89.97</v>
+        <v>90.449968217595199</v>
       </c>
       <c r="K124" s="3">
         <v>115.46622000000001</v>
@@ -5969,7 +5969,7 @@
         <v>91</v>
       </c>
       <c r="J125" s="3">
-        <v>90.85</v>
+        <v>90.693059466317294</v>
       </c>
       <c r="K125" s="3">
         <v>118.63722</v>
@@ -6017,7 +6017,7 @@
         <v>91.9</v>
       </c>
       <c r="J126" s="3">
-        <v>91.15</v>
+        <v>90.904414281105204</v>
       </c>
       <c r="K126" s="3">
         <v>120.4173</v>
@@ -6065,7 +6065,7 @@
         <v>89.9</v>
       </c>
       <c r="J127" s="3">
-        <v>91.73</v>
+        <v>91.308844983291706</v>
       </c>
       <c r="K127" s="3">
         <v>118.98238000000001</v>
@@ -6115,7 +6115,7 @@
         <v>91</v>
       </c>
       <c r="J128" s="3">
-        <v>92.08</v>
+        <v>91.6599010937598</v>
       </c>
       <c r="K128" s="3">
         <v>118.6477</v>
@@ -6163,7 +6163,7 @@
         <v>90.7</v>
       </c>
       <c r="J129" s="3">
-        <v>91.95</v>
+        <v>91.967366616255703</v>
       </c>
       <c r="K129" s="3">
         <v>118.4371</v>
@@ -6211,7 +6211,7 @@
         <v>91.5</v>
       </c>
       <c r="J130" s="3">
-        <v>91.82</v>
+        <v>91.882900541978699</v>
       </c>
       <c r="K130" s="3">
         <v>115.34504</v>
@@ -6261,7 +6261,7 @@
         <v>89.8</v>
       </c>
       <c r="J131" s="3">
-        <v>91.99</v>
+        <v>91.9620384472925</v>
       </c>
       <c r="K131" s="3">
         <v>114.35239</v>
@@ -6309,7 +6309,7 @@
         <v>87.6</v>
       </c>
       <c r="J132" s="3">
-        <v>92.02</v>
+        <v>91.937415607506296</v>
       </c>
       <c r="K132" s="3">
         <v>112.35907</v>
@@ -6357,7 +6357,7 @@
         <v>82.3</v>
       </c>
       <c r="J133" s="3">
-        <v>91.58</v>
+        <v>91.648176569292303</v>
       </c>
       <c r="K133" s="3">
         <v>112.00547</v>
@@ -6407,7 +6407,7 @@
         <v>79.599999999999994</v>
       </c>
       <c r="J134" s="3">
-        <v>91.46</v>
+        <v>91.431620223265796</v>
       </c>
       <c r="K134" s="3">
         <v>118.21059</v>
@@ -6455,7 +6455,7 @@
         <v>73.2</v>
       </c>
       <c r="J135" s="3">
-        <v>90.73</v>
+        <v>91.442149529848606</v>
       </c>
       <c r="K135" s="3">
         <v>119.64082000000001</v>
@@ -6503,7 +6503,7 @@
         <v>73</v>
       </c>
       <c r="J136" s="3">
-        <v>91.1</v>
+        <v>91.624215939207403</v>
       </c>
       <c r="K136" s="3">
         <v>118.35216</v>
@@ -6553,7 +6553,7 @@
         <v>71.599999999999994</v>
       </c>
       <c r="J137" s="3">
-        <v>91.44</v>
+        <v>91.359369123162196</v>
       </c>
       <c r="K137" s="3">
         <v>120.75400999999999</v>
@@ -6601,7 +6601,7 @@
         <v>73.099999999999994</v>
       </c>
       <c r="J138" s="3">
-        <v>91.76</v>
+        <v>91.376970400348895</v>
       </c>
       <c r="K138" s="3">
         <v>118.88688999999999</v>
@@ -6649,7 +6649,7 @@
         <v>73.400000000000006</v>
       </c>
       <c r="J139" s="3">
-        <v>91.81</v>
+        <v>91.413706605764602</v>
       </c>
       <c r="K139" s="3">
         <v>119.07429</v>
@@ -6699,7 +6699,7 @@
         <v>74.2</v>
       </c>
       <c r="J140" s="3">
-        <v>91.99</v>
+        <v>91.604652232639197</v>
       </c>
       <c r="K140" s="3">
         <v>119.74015</v>
@@ -6747,7 +6747,7 @@
         <v>77</v>
       </c>
       <c r="J141" s="3">
-        <v>91.39</v>
+        <v>91.507767279062094</v>
       </c>
       <c r="K141" s="3">
         <v>119.2996</v>
@@ -6795,7 +6795,7 @@
         <v>73.900000000000006</v>
       </c>
       <c r="J142" s="3">
-        <v>91.69</v>
+        <v>91.803260503037095</v>
       </c>
       <c r="K142" s="3">
         <v>118.17297000000001</v>
@@ -6845,7 +6845,7 @@
         <v>76</v>
       </c>
       <c r="J143" s="3">
-        <v>91.71</v>
+        <v>91.696840555146807</v>
       </c>
       <c r="K143" s="3">
         <v>119.84641999999999</v>
@@ -6893,7 +6893,7 @@
         <v>76.8</v>
       </c>
       <c r="J144" s="3">
-        <v>91.92</v>
+        <v>91.837307404482104</v>
       </c>
       <c r="K144" s="3">
         <v>120.50859</v>
@@ -6941,7 +6941,7 @@
         <v>77.099999999999994</v>
       </c>
       <c r="J145" s="3">
-        <v>92.02</v>
+        <v>92.080767198345299</v>
       </c>
       <c r="K145" s="3">
         <v>120.19752</v>
@@ -6991,7 +6991,7 @@
         <v>78.599999999999994</v>
       </c>
       <c r="J146" s="3">
-        <v>92.3</v>
+        <v>92.225199392899498</v>
       </c>
       <c r="K146" s="3">
         <v>118.95456</v>
@@ -7039,7 +7039,7 @@
         <v>78.400000000000006</v>
       </c>
       <c r="J147" s="3">
-        <v>91.57</v>
+        <v>92.308932914453095</v>
       </c>
       <c r="K147" s="3">
         <v>116.52484</v>
@@ -7087,7 +7087,7 @@
         <v>79.900000000000006</v>
       </c>
       <c r="J148" s="3">
-        <v>91.85</v>
+        <v>92.3866131926804</v>
       </c>
       <c r="K148" s="3">
         <v>112.43545</v>
@@ -7137,7 +7137,7 @@
         <v>83.8</v>
       </c>
       <c r="J149" s="3">
-        <v>92.86</v>
+        <v>92.666598308030402</v>
       </c>
       <c r="K149" s="3">
         <v>111.46167</v>
@@ -7185,7 +7185,7 @@
         <v>82.5</v>
       </c>
       <c r="J150" s="3">
-        <v>93.24</v>
+        <v>92.765707207847299</v>
       </c>
       <c r="K150" s="3">
         <v>110.30087</v>
@@ -7233,7 +7233,7 @@
         <v>84.8</v>
       </c>
       <c r="J151" s="3">
-        <v>93.35</v>
+        <v>92.920135762051004</v>
       </c>
       <c r="K151" s="3">
         <v>106.96250000000001</v>
@@ -7283,7 +7283,7 @@
         <v>86.7</v>
       </c>
       <c r="J152" s="3">
-        <v>93.35</v>
+        <v>92.985593236201495</v>
       </c>
       <c r="K152" s="3">
         <v>104.92502</v>
@@ -7331,7 +7331,7 @@
         <v>88.3</v>
       </c>
       <c r="J153" s="3">
-        <v>92.96</v>
+        <v>93.165199800064201</v>
       </c>
       <c r="K153" s="3">
         <v>106.97564</v>
@@ -7379,7 +7379,7 @@
         <v>87.5</v>
       </c>
       <c r="J154" s="3">
-        <v>93.13</v>
+        <v>93.313509982295201</v>
       </c>
       <c r="K154" s="3">
         <v>106.06599</v>
@@ -7429,7 +7429,7 @@
         <v>87.8</v>
       </c>
       <c r="J155" s="3">
-        <v>93.42</v>
+        <v>93.405738754823801</v>
       </c>
       <c r="K155" s="3">
         <v>106.66743</v>
@@ -7477,7 +7477,7 @@
         <v>90.3</v>
       </c>
       <c r="J156" s="3">
-        <v>93.7</v>
+        <v>93.617358657251401</v>
       </c>
       <c r="K156" s="3">
         <v>110.41763</v>
@@ -7525,7 +7525,7 @@
         <v>89.4</v>
       </c>
       <c r="J157" s="3">
-        <v>93.79</v>
+        <v>93.856676162756699</v>
       </c>
       <c r="K157" s="3">
         <v>108.99939000000001</v>
@@ -7575,7 +7575,7 @@
         <v>86.5</v>
       </c>
       <c r="J158" s="3">
-        <v>94.35</v>
+        <v>94.245456040980201</v>
       </c>
       <c r="K158" s="3">
         <v>106.47226000000001</v>
@@ -7623,7 +7623,7 @@
         <v>90.1</v>
       </c>
       <c r="J159" s="3">
-        <v>93.69</v>
+        <v>94.485093995564995</v>
       </c>
       <c r="K159" s="3">
         <v>106.59511999999999</v>
@@ -7671,7 +7671,7 @@
         <v>91.5</v>
       </c>
       <c r="J160" s="3">
-        <v>94.08</v>
+        <v>94.654546464786094</v>
       </c>
       <c r="K160" s="3">
         <v>106.65206999999999</v>
@@ -7721,7 +7721,7 @@
         <v>91.3</v>
       </c>
       <c r="J161" s="3">
-        <v>95.35</v>
+        <v>95.071942968696703</v>
       </c>
       <c r="K161" s="3">
         <v>108.46178999999999</v>
@@ -7769,7 +7769,7 @@
         <v>92.5</v>
       </c>
       <c r="J162" s="3">
-        <v>95.88</v>
+        <v>95.330032504782295</v>
       </c>
       <c r="K162" s="3">
         <v>110.55079000000001</v>
@@ -7817,7 +7817,7 @@
         <v>91.3</v>
       </c>
       <c r="J163" s="3">
-        <v>95.89</v>
+        <v>95.438007655586901</v>
       </c>
       <c r="K163" s="3">
         <v>109.61203</v>
@@ -7867,7 +7867,7 @@
         <v>91.6</v>
       </c>
       <c r="J164" s="3">
-        <v>95.88</v>
+        <v>95.529300858664996</v>
       </c>
       <c r="K164" s="3">
         <v>109.51108000000001</v>
@@ -7915,7 +7915,7 @@
         <v>93.2</v>
       </c>
       <c r="J165" s="3">
-        <v>95.34</v>
+        <v>95.608772541830405</v>
       </c>
       <c r="K165" s="3">
         <v>108.53318</v>
@@ -7963,7 +7963,7 @@
         <v>93.8</v>
       </c>
       <c r="J166" s="3">
-        <v>95.52</v>
+        <v>95.749497103616093</v>
       </c>
       <c r="K166" s="3">
         <v>108.62390000000001</v>
@@ -8013,7 +8013,7 @@
         <v>92.9</v>
       </c>
       <c r="J167" s="3">
-        <v>96.21</v>
+        <v>96.140547790804703</v>
       </c>
       <c r="K167" s="3">
         <v>108.0919</v>
@@ -8061,7 +8061,7 @@
         <v>91.8</v>
       </c>
       <c r="J168" s="3">
-        <v>96.54</v>
+        <v>96.410324834497999</v>
       </c>
       <c r="K168" s="3">
         <v>108.79506000000001</v>
@@ -8109,7 +8109,7 @@
         <v>93.4</v>
       </c>
       <c r="J169" s="3">
-        <v>96.63</v>
+        <v>96.679835481745997</v>
       </c>
       <c r="K169" s="3">
         <v>108.0099</v>
@@ -8159,7 +8159,7 @@
         <v>93.5</v>
       </c>
       <c r="J170" s="3">
-        <v>96.95</v>
+        <v>96.823466962513294</v>
       </c>
       <c r="K170" s="3">
         <v>106.22983000000001</v>
@@ -8207,7 +8207,7 @@
         <v>93.5</v>
       </c>
       <c r="J171" s="3">
-        <v>96.17</v>
+        <v>97.042106221143499</v>
       </c>
       <c r="K171" s="3">
         <v>104.13615</v>
@@ -8255,7 +8255,7 @@
         <v>93.6</v>
       </c>
       <c r="J172" s="3">
-        <v>96.65</v>
+        <v>97.2753514928594</v>
       </c>
       <c r="K172" s="3">
         <v>103.43059</v>
@@ -8305,7 +8305,7 @@
         <v>94.9</v>
       </c>
       <c r="J173" s="3">
-        <v>97.9</v>
+        <v>97.602413553127803</v>
       </c>
       <c r="K173" s="3">
         <v>104.09802999999999</v>
@@ -8353,7 +8353,7 @@
         <v>94.6</v>
       </c>
       <c r="J174" s="3">
-        <v>98.36</v>
+        <v>97.8055950094775</v>
       </c>
       <c r="K174" s="3">
         <v>104.39406</v>
@@ -8401,7 +8401,7 @@
         <v>96.8</v>
       </c>
       <c r="J175" s="3">
-        <v>98.23</v>
+        <v>97.7912077463305</v>
       </c>
       <c r="K175" s="3">
         <v>103.41569</v>
@@ -8451,7 +8451,7 @@
         <v>96.2</v>
       </c>
       <c r="J176" s="3">
-        <v>98.16</v>
+        <v>97.809445806633207</v>
       </c>
       <c r="K176" s="3">
         <v>102.84652</v>
@@ -8499,7 +8499,7 @@
         <v>95.4</v>
       </c>
       <c r="J177" s="3">
-        <v>97.64</v>
+        <v>97.924194709024505</v>
       </c>
       <c r="K177" s="3">
         <v>100.58271000000001</v>
@@ -8547,7 +8547,7 @@
         <v>98.9</v>
       </c>
       <c r="J178" s="3">
-        <v>98.02</v>
+        <v>98.237787112438198</v>
       </c>
       <c r="K178" s="3">
         <v>99.899709999999999</v>
@@ -8597,7 +8597,7 @@
         <v>96</v>
       </c>
       <c r="J179" s="3">
-        <v>98.73</v>
+        <v>98.582094432766894</v>
       </c>
       <c r="K179" s="3">
         <v>102.38182999999999</v>
@@ -8645,7 +8645,7 @@
         <v>95.4</v>
       </c>
       <c r="J180" s="3">
-        <v>98.96</v>
+        <v>98.775897944378798</v>
       </c>
       <c r="K180" s="3">
         <v>103.16244</v>
@@ -8693,7 +8693,7 @@
         <v>94.9</v>
       </c>
       <c r="J181" s="3">
-        <v>98.76</v>
+        <v>98.792268682193495</v>
       </c>
       <c r="K181" s="3">
         <v>102.4606</v>
@@ -8743,7 +8743,7 @@
         <v>96.1</v>
       </c>
       <c r="J182" s="3">
-        <v>99.11</v>
+        <v>98.967009112764501</v>
       </c>
       <c r="K182" s="3">
         <v>103.68454</v>
@@ -8791,7 +8791,7 @@
         <v>96</v>
       </c>
       <c r="J183" s="3">
-        <v>98.09</v>
+        <v>99.044680352705896</v>
       </c>
       <c r="K183" s="3">
         <v>105.32942</v>
@@ -8839,7 +8839,7 @@
         <v>95.9</v>
       </c>
       <c r="J184" s="3">
-        <v>98.45</v>
+        <v>99.132653424014507</v>
       </c>
       <c r="K184" s="3">
         <v>105.38652</v>
@@ -8889,7 +8889,7 @@
         <v>99.2</v>
       </c>
       <c r="J185" s="3">
-        <v>99.61</v>
+        <v>99.216417714706793</v>
       </c>
       <c r="K185" s="3">
         <v>103.84202999999999</v>
@@ -8937,7 +8937,7 @@
         <v>97.2</v>
       </c>
       <c r="J186" s="3">
-        <v>99.52</v>
+        <v>99.14064561571</v>
       </c>
       <c r="K186" s="3">
         <v>104.96845999999999</v>
@@ -8985,7 +8985,7 @@
         <v>96.8</v>
       </c>
       <c r="J187" s="3">
-        <v>99.63</v>
+        <v>99.200637834134298</v>
       </c>
       <c r="K187" s="3">
         <v>104.83443</v>
@@ -9035,7 +9035,7 @@
         <v>96.5</v>
       </c>
       <c r="J188" s="3">
-        <v>99.74</v>
+        <v>99.347818488439501</v>
       </c>
       <c r="K188" s="3">
         <v>106.92223</v>
@@ -9083,7 +9083,7 @@
         <v>96.9</v>
       </c>
       <c r="J189" s="3">
-        <v>99.21</v>
+        <v>99.444700207679702</v>
       </c>
       <c r="K189" s="3">
         <v>106.92659999999999</v>
@@ -9131,7 +9131,7 @@
         <v>98.9</v>
       </c>
       <c r="J190" s="3">
-        <v>99.33</v>
+        <v>99.497528748953997</v>
       </c>
       <c r="K190" s="3">
         <v>107.49525</v>
@@ -9181,7 +9181,7 @@
         <v>97.2</v>
       </c>
       <c r="J191" s="3">
-        <v>99.81</v>
+        <v>99.606951725166397</v>
       </c>
       <c r="K191" s="3">
         <v>107.31641999999999</v>
@@ -9229,7 +9229,7 @@
         <v>97.4</v>
       </c>
       <c r="J192" s="3">
-        <v>99.69</v>
+        <v>99.481981225300402</v>
       </c>
       <c r="K192" s="3">
         <v>108.30383999999999</v>
@@ -9277,7 +9277,7 @@
         <v>97.3</v>
       </c>
       <c r="J193" s="3">
-        <v>99.6</v>
+        <v>99.633019169904401</v>
       </c>
       <c r="K193" s="3">
         <v>107.88202</v>
@@ -9327,7 +9327,7 @@
         <v>96.9</v>
       </c>
       <c r="J194" s="3">
-        <v>99.95</v>
+        <v>99.825212218650094</v>
       </c>
       <c r="K194" s="3">
         <v>109.34529000000001</v>
@@ -9375,7 +9375,7 @@
         <v>97.7</v>
       </c>
       <c r="J195" s="3">
-        <v>98.84</v>
+        <v>99.893276580863798</v>
       </c>
       <c r="K195" s="3">
         <v>109.65510999999999</v>
@@ -9423,7 +9423,7 @@
         <v>99.1</v>
       </c>
       <c r="J196" s="3">
-        <v>99.14</v>
+        <v>99.893001785471199</v>
       </c>
       <c r="K196" s="3">
         <v>108.93977</v>
@@ -9473,7 +9473,7 @@
         <v>96.7</v>
       </c>
       <c r="J197" s="3">
-        <v>100.07</v>
+        <v>99.865356704558096</v>
       </c>
       <c r="K197" s="3">
         <v>110.42899</v>
@@ -9521,7 +9521,7 @@
         <v>98.2</v>
       </c>
       <c r="J198" s="3">
-        <v>100.22</v>
+        <v>99.742503058889795</v>
       </c>
       <c r="K198" s="3">
         <v>110.16345</v>
@@ -9569,7 +9569,7 @@
         <v>98.7</v>
       </c>
       <c r="J199" s="3">
-        <v>100.12</v>
+        <v>99.6633868656141</v>
       </c>
       <c r="K199" s="3">
         <v>108.8051</v>
@@ -9619,7 +9619,7 @@
         <v>98.6</v>
       </c>
       <c r="J200" s="3">
-        <v>100.23</v>
+        <v>99.770623745370798</v>
       </c>
       <c r="K200" s="3">
         <v>107.44788</v>
@@ -9667,7 +9667,7 @@
         <v>99</v>
       </c>
       <c r="J201" s="3">
-        <v>99.58</v>
+        <v>99.733437536499196</v>
       </c>
       <c r="K201" s="3">
         <v>106.91784</v>
@@ -9715,7 +9715,7 @@
         <v>97.2</v>
       </c>
       <c r="J202" s="3">
-        <v>99.69</v>
+        <v>99.788927613686695</v>
       </c>
       <c r="K202" s="3">
         <v>105.77665</v>
@@ -9765,7 +9765,7 @@
         <v>99.8</v>
       </c>
       <c r="J203" s="3">
-        <v>100.13</v>
+        <v>99.886400089292493</v>
       </c>
       <c r="K203" s="3">
         <v>104.6648</v>
@@ -9813,7 +9813,7 @@
         <v>99.9</v>
       </c>
       <c r="J204" s="3">
-        <v>100.06</v>
+        <v>99.808276850825294</v>
       </c>
       <c r="K204" s="3">
         <v>104.74021</v>
@@ -9861,7 +9861,7 @@
         <v>99</v>
       </c>
       <c r="J205" s="3">
-        <v>99.88</v>
+        <v>99.919519322979099</v>
       </c>
       <c r="K205" s="3">
         <v>105.08802</v>
@@ -9911,7 +9911,7 @@
         <v>101.1</v>
       </c>
       <c r="J206" s="3">
-        <v>99.78</v>
+        <v>99.7034690348124</v>
       </c>
       <c r="K206" s="3">
         <v>106.9221</v>
@@ -9959,7 +9959,7 @@
         <v>99.7</v>
       </c>
       <c r="J207" s="3">
-        <v>98.24</v>
+        <v>99.393074673155198</v>
       </c>
       <c r="K207" s="3">
         <v>103.25819</v>
@@ -10007,7 +10007,7 @@
         <v>100.8</v>
       </c>
       <c r="J208" s="3">
-        <v>98.85</v>
+        <v>99.699851085821393</v>
       </c>
       <c r="K208" s="3">
         <v>100.15781</v>
@@ -10057,7 +10057,7 @@
         <v>99.6</v>
       </c>
       <c r="J209" s="3">
-        <v>100</v>
+        <v>99.887314910080207</v>
       </c>
       <c r="K209" s="3">
         <v>97.230930000000001</v>
@@ -10105,7 +10105,7 @@
         <v>101.3</v>
       </c>
       <c r="J210" s="3">
-        <v>100.43</v>
+        <v>99.977152192705006</v>
       </c>
       <c r="K210" s="3">
         <v>96.141069999999999</v>
@@ -10153,7 +10153,7 @@
         <v>101.5</v>
       </c>
       <c r="J211" s="3">
-        <v>100.71</v>
+        <v>100.207964594332</v>
       </c>
       <c r="K211" s="3">
         <v>98.234889999999993</v>
@@ -10203,7 +10203,7 @@
         <v>100.3</v>
       </c>
       <c r="J212" s="3">
-        <v>100.72</v>
+        <v>100.19457954827</v>
       </c>
       <c r="K212" s="3">
         <v>99.762439999999998</v>
@@ -10251,7 +10251,7 @@
         <v>102</v>
       </c>
       <c r="J213" s="3">
-        <v>100.12</v>
+        <v>100.186915003061</v>
       </c>
       <c r="K213" s="3">
         <v>98.803659999999994</v>
@@ -10299,7 +10299,7 @@
         <v>97.9</v>
       </c>
       <c r="J214" s="3">
-        <v>100.12</v>
+        <v>100.153206506579</v>
       </c>
       <c r="K214" s="3">
         <v>101.27927</v>
@@ -10349,7 +10349,7 @@
         <v>98.3</v>
       </c>
       <c r="J215" s="3">
-        <v>100.32</v>
+        <v>100.055302357835</v>
       </c>
       <c r="K215" s="3">
         <v>102.92628999999999</v>
@@ -10397,7 +10397,7 @@
         <v>100.5</v>
       </c>
       <c r="J216" s="3">
-        <v>100.45</v>
+        <v>100.150135088832</v>
       </c>
       <c r="K216" s="3">
         <v>102.39060000000001</v>
@@ -10445,7 +10445,7 @@
         <v>99</v>
       </c>
       <c r="J217" s="3">
-        <v>100.01</v>
+        <v>100.065321780094</v>
       </c>
       <c r="K217" s="3">
         <v>99.209540000000004</v>
@@ -10495,7 +10495,7 @@
         <v>99.1</v>
       </c>
       <c r="J218" s="3">
-        <v>100.03</v>
+        <v>99.968524665310198</v>
       </c>
       <c r="K218" s="3">
         <v>100.88139</v>
@@ -10543,7 +10543,7 @@
         <v>99.3</v>
       </c>
       <c r="J219" s="3">
-        <v>98.56</v>
+        <v>99.712881208923406</v>
       </c>
       <c r="K219" s="3">
         <v>102.87944</v>
@@ -10591,7 +10591,7 @@
         <v>98.6</v>
       </c>
       <c r="J220" s="3">
-        <v>98.72</v>
+        <v>99.602378409730406</v>
       </c>
       <c r="K220" s="3">
         <v>102.96245</v>
@@ -10641,7 +10641,7 @@
         <v>100.9</v>
       </c>
       <c r="J221" s="3">
-        <v>99.95</v>
+        <v>99.784198280389703</v>
       </c>
       <c r="K221" s="3">
         <v>101.61870999999999</v>
@@ -10689,7 +10689,7 @@
         <v>101.9</v>
       </c>
       <c r="J222" s="3">
-        <v>100.17</v>
+        <v>99.879813917073506</v>
       </c>
       <c r="K222" s="3">
         <v>103.19364</v>
@@ -10737,7 +10737,7 @@
         <v>99.2</v>
       </c>
       <c r="J223" s="3">
-        <v>100.58</v>
+        <v>100.09362913458</v>
       </c>
       <c r="K223" s="3">
         <v>103.3901</v>
@@ -10787,7 +10787,7 @@
         <v>99.9</v>
       </c>
       <c r="J224" s="3">
-        <v>100.76</v>
+        <v>100.24051974580399</v>
       </c>
       <c r="K224" s="3">
         <v>103.26246</v>
@@ -10835,7 +10835,7 @@
         <v>100</v>
       </c>
       <c r="J225" s="3">
-        <v>100.28</v>
+        <v>100.32203432934099</v>
       </c>
       <c r="K225" s="3">
         <v>103.11108</v>
@@ -10883,7 +10883,7 @@
         <v>101.4</v>
       </c>
       <c r="J226" s="3">
-        <v>100.34</v>
+        <v>100.358857195319</v>
       </c>
       <c r="K226" s="3">
         <v>103.11096000000001</v>
@@ -10933,7 +10933,7 @@
         <v>100.6</v>
       </c>
       <c r="J227" s="3">
-        <v>100.71</v>
+        <v>100.46074623472801</v>
       </c>
       <c r="K227" s="3">
         <v>103.41455000000001</v>
@@ -10981,7 +10981,7 @@
         <v>100.1</v>
       </c>
       <c r="J228" s="3">
-        <v>100.95</v>
+        <v>100.650528695688</v>
       </c>
       <c r="K228" s="3">
         <v>103.43071</v>
@@ -11029,7 +11029,7 @@
         <v>101.7</v>
       </c>
       <c r="J229" s="3">
-        <v>100.59</v>
+        <v>100.68800906630599</v>
       </c>
       <c r="K229" s="3">
         <v>103.00412</v>
@@ -11079,7 +11079,7 @@
         <v>103.8</v>
       </c>
       <c r="J230" s="3">
-        <v>101.12</v>
+        <v>101.071348364481</v>
       </c>
       <c r="K230" s="3">
         <v>101.32931000000001</v>
@@ -11127,7 +11127,7 @@
         <v>101</v>
       </c>
       <c r="J231" s="3">
-        <v>100.26</v>
+        <v>101.35115041089</v>
       </c>
       <c r="K231" s="3">
         <v>102.11313</v>
@@ -11175,7 +11175,7 @@
         <v>103.5</v>
       </c>
       <c r="J232" s="3">
-        <v>100.65</v>
+        <v>101.495447738246</v>
       </c>
       <c r="K232" s="3">
         <v>100.15033</v>
@@ -11225,7 +11225,7 @@
         <v>104.7</v>
       </c>
       <c r="J233" s="3">
-        <v>101.48</v>
+        <v>101.459386792782</v>
       </c>
       <c r="K233" s="3">
         <v>101.09523</v>
@@ -11273,7 +11273,7 @@
         <v>103.7</v>
       </c>
       <c r="J234" s="3">
-        <v>102.06</v>
+        <v>101.620597143461</v>
       </c>
       <c r="K234" s="3">
         <v>101.15716999999999</v>
@@ -11321,7 +11321,7 @@
         <v>105.8</v>
       </c>
       <c r="J235" s="3">
-        <v>101.97</v>
+        <v>101.48272257126099</v>
       </c>
       <c r="K235" s="3">
         <v>103.62282</v>
@@ -11371,7 +11371,7 @@
         <v>104.2</v>
       </c>
       <c r="J236" s="3">
-        <v>102.07</v>
+        <v>101.55146029901501</v>
       </c>
       <c r="K236" s="3">
         <v>104.41273</v>
@@ -11419,7 +11419,7 @@
         <v>103.2</v>
       </c>
       <c r="J237" s="3">
-        <v>101.62</v>
+        <v>101.636160365252</v>
       </c>
       <c r="K237" s="3">
         <v>106.14952</v>
@@ -11467,7 +11467,7 @@
         <v>106.2</v>
       </c>
       <c r="J238" s="3">
-        <v>101.88</v>
+        <v>101.878334701437</v>
       </c>
       <c r="K238" s="3">
         <v>107.44028</v>
@@ -11517,7 +11517,7 @@
         <v>107.2</v>
       </c>
       <c r="J239" s="3">
-        <v>102.29</v>
+        <v>102.03847469462001</v>
       </c>
       <c r="K239" s="3">
         <v>107.46003</v>
@@ -11565,7 +11565,7 @@
         <v>103.2</v>
       </c>
       <c r="J240" s="3">
-        <v>102.34</v>
+        <v>102.036078769504</v>
       </c>
       <c r="K240" s="3">
         <v>107.31335</v>
@@ -11613,7 +11613,7 @@
         <v>107.6</v>
       </c>
       <c r="J241" s="3">
-        <v>102.13</v>
+        <v>102.26299761132501</v>
       </c>
       <c r="K241" s="3">
         <v>107.39887</v>
@@ -11663,7 +11663,7 @@
         <v>111</v>
       </c>
       <c r="J242" s="3">
-        <v>102.48</v>
+        <v>102.494149692646</v>
       </c>
       <c r="K242" s="3">
         <v>107.25282</v>
@@ -11711,7 +11711,7 @@
         <v>109</v>
       </c>
       <c r="J243" s="3">
-        <v>101.55</v>
+        <v>102.637043786619</v>
       </c>
       <c r="K243" s="3">
         <v>108.26183</v>
@@ -11759,7 +11759,7 @@
         <v>106</v>
       </c>
       <c r="J244" s="3">
-        <v>101.77</v>
+        <v>102.621792411464</v>
       </c>
       <c r="K244" s="3">
         <v>107.71727</v>
@@ -11809,7 +11809,7 @@
         <v>108</v>
       </c>
       <c r="J245" s="3">
-        <v>102.9</v>
+        <v>102.787720188251</v>
       </c>
       <c r="K245" s="3">
         <v>107.94855</v>
@@ -11857,7 +11857,7 @@
         <v>106.9</v>
       </c>
       <c r="J246" s="3">
-        <v>103.32</v>
+        <v>103.029909045181</v>
       </c>
       <c r="K246" s="3">
         <v>109.17753</v>
@@ -11905,7 +11905,7 @@
         <v>106.5</v>
       </c>
       <c r="J247" s="3">
-        <v>103.96</v>
+        <v>103.46743236960199</v>
       </c>
       <c r="K247" s="3">
         <v>108.00145000000001</v>
@@ -11955,7 +11955,7 @@
         <v>109.1</v>
       </c>
       <c r="J248" s="3">
-        <v>104.08</v>
+        <v>103.53589551831899</v>
       </c>
       <c r="K248" s="3">
         <v>108.3725</v>
@@ -12003,7 +12003,7 @@
         <v>105.8</v>
       </c>
       <c r="J249" s="3">
-        <v>103.85</v>
+        <v>103.80916169986099</v>
       </c>
       <c r="K249" s="3">
         <v>109.30714</v>
@@ -12051,7 +12051,7 @@
         <v>108.3</v>
       </c>
       <c r="J250" s="3">
-        <v>104</v>
+        <v>103.96041774608</v>
       </c>
       <c r="K250" s="3">
         <v>109.8741</v>
@@ -12101,7 +12101,7 @@
         <v>106.5</v>
       </c>
       <c r="J251" s="3">
-        <v>104.41</v>
+        <v>104.14708062615099</v>
       </c>
       <c r="K251" s="3">
         <v>110.95663999999999</v>
@@ -12149,7 +12149,7 @@
         <v>106.8</v>
       </c>
       <c r="J252" s="3">
-        <v>104.67</v>
+        <v>104.33776803185</v>
       </c>
       <c r="K252" s="3">
         <v>109.25174</v>
@@ -12197,7 +12197,7 @@
         <v>106.1</v>
       </c>
       <c r="J253" s="3">
-        <v>104.09</v>
+        <v>104.232300425586</v>
       </c>
       <c r="K253" s="3">
         <v>108.20818</v>
@@ -12247,7 +12247,7 @@
         <v>107.3</v>
       </c>
       <c r="J254" s="3">
-        <v>104.04</v>
+        <v>104.10831081269301</v>
       </c>
       <c r="K254" s="3">
         <v>108.01441</v>
@@ -12295,7 +12295,7 @@
         <v>107.4</v>
       </c>
       <c r="J255" s="3">
-        <v>102.96</v>
+        <v>104.030749249816</v>
       </c>
       <c r="K255" s="3">
         <v>107.51721999999999</v>
@@ -12343,7 +12343,7 @@
         <v>107.6</v>
       </c>
       <c r="J256" s="3">
-        <v>103.28</v>
+        <v>104.090953141513</v>
       </c>
       <c r="K256" s="3">
         <v>105.89451</v>
@@ -12393,7 +12393,7 @@
         <v>108.7</v>
       </c>
       <c r="J257" s="3">
-        <v>104.34</v>
+        <v>104.359697762594</v>
       </c>
       <c r="K257" s="3">
         <v>105.58177999999999</v>
@@ -12441,7 +12441,7 @@
         <v>105.6</v>
       </c>
       <c r="J258" s="3">
-        <v>105.09</v>
+        <v>104.670785025714</v>
       </c>
       <c r="K258" s="3">
         <v>106.0134</v>
@@ -12489,7 +12489,7 @@
         <v>106.8</v>
       </c>
       <c r="J259" s="3">
-        <v>105.23</v>
+        <v>104.769798698819</v>
       </c>
       <c r="K259" s="3">
         <v>107.04437</v>
@@ -12539,7 +12539,7 @@
         <v>106.4</v>
       </c>
       <c r="J260" s="3">
-        <v>105.4</v>
+        <v>104.854334298609</v>
       </c>
       <c r="K260" s="3">
         <v>107.36648</v>
@@ -12587,7 +12587,7 @@
         <v>105.7</v>
       </c>
       <c r="J261" s="3">
-        <v>104.91</v>
+        <v>104.853330043713</v>
       </c>
       <c r="K261" s="3">
         <v>106.64875000000001</v>
@@ -12635,7 +12635,7 @@
         <v>107.2</v>
       </c>
       <c r="J262" s="3">
-        <v>105.05</v>
+        <v>105.036077295109</v>
       </c>
       <c r="K262" s="3">
         <v>106.87461999999999</v>
@@ -12685,7 +12685,7 @@
         <v>106.1</v>
       </c>
       <c r="J263" s="3">
-        <v>105.28</v>
+        <v>105.08256652771399</v>
       </c>
       <c r="K263" s="3">
         <v>106.06104000000001</v>
@@ -12733,7 +12733,7 @@
         <v>108.4</v>
       </c>
       <c r="J264" s="3">
-        <v>105.43</v>
+        <v>105.13788762472799</v>
       </c>
       <c r="K264" s="3">
         <v>106.00530999999999</v>
@@ -12781,7 +12781,7 @@
         <v>105.5</v>
       </c>
       <c r="J265" s="3">
-        <v>105.09</v>
+        <v>105.262090283986</v>
       </c>
       <c r="K265" s="3">
         <v>105.11144</v>
@@ -12831,7 +12831,7 @@
         <v>106.1</v>
       </c>
       <c r="J266" s="3">
-        <v>105.42</v>
+        <v>105.53244869608901</v>
       </c>
       <c r="K266" s="3">
         <v>104.52836000000001</v>
@@ -12879,7 +12879,7 @@
         <v>105.6</v>
       </c>
       <c r="J267" s="3">
-        <v>104.37</v>
+        <v>105.351605874656</v>
       </c>
       <c r="K267" s="3">
         <v>104.34526</v>
@@ -12927,7 +12927,7 @@
         <v>106</v>
       </c>
       <c r="J268" s="3">
-        <v>104.55</v>
+        <v>105.213584077934</v>
       </c>
       <c r="K268" s="3">
         <v>102.58183</v>
@@ -12977,7 +12977,7 @@
         <v>96.9</v>
       </c>
       <c r="J269" s="3">
-        <v>105.12</v>
+        <v>105.06285375588099</v>
       </c>
       <c r="K269" s="3">
         <v>106.87915</v>
@@ -13025,7 +13025,7 @@
         <v>74.099999999999994</v>
       </c>
       <c r="J270" s="3">
-        <v>105.42</v>
+        <v>104.98722544066</v>
       </c>
       <c r="K270" s="3">
         <v>107.05676</v>
@@ -13073,7 +13073,7 @@
         <v>81.099999999999994</v>
       </c>
       <c r="J271" s="3">
-        <v>105.32</v>
+        <v>104.892046844879</v>
       </c>
       <c r="K271" s="3">
         <v>107.83749</v>
@@ -13123,7 +13123,7 @@
         <v>89</v>
       </c>
       <c r="J272" s="3">
-        <v>105.68</v>
+        <v>105.148251514801</v>
       </c>
       <c r="K272" s="3">
         <v>109.04156</v>
@@ -13171,7 +13171,7 @@
         <v>96.2</v>
       </c>
       <c r="J273" s="3">
-        <v>105.31</v>
+        <v>105.250501041927</v>
       </c>
       <c r="K273" s="3">
         <v>110.25254</v>
@@ -13219,7 +13219,7 @@
         <v>97.6</v>
       </c>
       <c r="J274" s="3">
-        <v>104.87</v>
+        <v>104.890734584923</v>
       </c>
       <c r="K274" s="3">
         <v>111.63551</v>
@@ -13269,7 +13269,7 @@
         <v>101.8</v>
       </c>
       <c r="J275" s="3">
-        <v>104.95</v>
+        <v>104.830650455317</v>
       </c>
       <c r="K275" s="3">
         <v>110.92238999999999</v>
@@ -13317,7 +13317,7 @@
         <v>103.5</v>
       </c>
       <c r="J276" s="3">
-        <v>105.14</v>
+        <v>104.924152089548</v>
       </c>
       <c r="K276" s="3">
         <v>111.00416</v>
@@ -13365,7 +13365,7 @@
         <v>104.5</v>
       </c>
       <c r="J277" s="3">
-        <v>104.79</v>
+        <v>105.03103134341301</v>
       </c>
       <c r="K277" s="3">
         <v>110.20014</v>
@@ -13415,7 +13415,7 @@
         <v>104.4</v>
       </c>
       <c r="J278" s="3">
-        <v>105.13</v>
+        <v>105.37509881398699</v>
       </c>
       <c r="K278" s="3">
         <v>110.78273</v>
@@ -13463,7 +13463,7 @@
         <v>104</v>
       </c>
       <c r="J279" s="3">
-        <v>105.31</v>
+        <v>106.24916231087499</v>
       </c>
       <c r="K279" s="3">
         <v>110.35332</v>
@@ -13511,7 +13511,7 @@
         <v>104.1</v>
       </c>
       <c r="J280" s="3">
-        <v>105.53</v>
+        <v>106.066589054274</v>
       </c>
       <c r="K280" s="3">
         <v>109.33111</v>
@@ -13561,7 +13561,7 @@
         <v>104.7</v>
       </c>
       <c r="J281" s="3">
-        <v>106.52</v>
+        <v>106.385823692627</v>
       </c>
       <c r="K281" s="3">
         <v>109.24885999999999</v>
@@ -13609,7 +13609,7 @@
         <v>105</v>
       </c>
       <c r="J282" s="3">
-        <v>107.12</v>
+        <v>106.666832324287</v>
       </c>
       <c r="K282" s="3">
         <v>110.31981</v>
@@ -13657,7 +13657,7 @@
         <v>104.4</v>
       </c>
       <c r="J283" s="3">
-        <v>107.4</v>
+        <v>106.978995878229</v>
       </c>
       <c r="K283" s="3">
         <v>110.68707000000001</v>
@@ -13707,7 +13707,7 @@
         <v>103.6</v>
       </c>
       <c r="J284" s="3">
-        <v>107.69</v>
+        <v>107.18000908822199</v>
       </c>
       <c r="K284" s="3">
         <v>109.75100999999999</v>
@@ -13755,7 +13755,7 @@
         <v>104.5</v>
       </c>
       <c r="J285" s="3">
-        <v>107.6</v>
+        <v>107.55983978162401</v>
       </c>
       <c r="K285" s="3">
         <v>108.88347</v>
@@ -13803,7 +13803,7 @@
         <v>102.7</v>
       </c>
       <c r="J286" s="3">
-        <v>107.97</v>
+        <v>107.977777893799</v>
       </c>
       <c r="K286" s="3">
         <v>107.88037</v>
@@ -13853,7 +13853,7 @@
         <v>102.3</v>
       </c>
       <c r="J287" s="3">
-        <v>108.48</v>
+        <v>108.340364212997</v>
       </c>
       <c r="K287" s="3">
         <v>108.11903</v>
@@ -13901,7 +13901,7 @@
         <v>103.8</v>
       </c>
       <c r="J288" s="3">
-        <v>109.4</v>
+        <v>109.167320783619</v>
       </c>
       <c r="K288" s="3">
         <v>107.52208</v>
@@ -13949,7 +13949,7 @@
         <v>105.6</v>
       </c>
       <c r="J289" s="3">
-        <v>109.89</v>
+        <v>110.16096055012601</v>
       </c>
       <c r="K289" s="3">
         <v>107.14761</v>
@@ -13999,7 +13999,7 @@
         <v>103.3</v>
       </c>
       <c r="J290" s="3">
-        <v>110.36</v>
+        <v>110.759595454188</v>
       </c>
       <c r="K290" s="3">
         <v>107.46392</v>
@@ -14047,7 +14047,7 @@
         <v>109.5</v>
       </c>
       <c r="J291" s="3">
-        <v>110.69</v>
+        <v>111.670085580444</v>
       </c>
       <c r="K291" s="3">
         <v>106.97842</v>
@@ -14095,7 +14095,7 @@
         <v>107.7</v>
       </c>
       <c r="J292" s="3">
-        <v>111.73</v>
+        <v>112.218967193848</v>
       </c>
       <c r="K292" s="3">
         <v>106.84659000000001</v>
@@ -14145,7 +14145,7 @@
         <v>103.9</v>
       </c>
       <c r="J293" s="3">
-        <v>114.45</v>
+        <v>114.276310181789</v>
       </c>
       <c r="K293" s="3">
         <v>107.28316</v>
@@ -14193,7 +14193,7 @@
         <v>106.2</v>
       </c>
       <c r="J294" s="3">
-        <v>115.11</v>
+        <v>114.619726960086</v>
       </c>
       <c r="K294" s="3">
         <v>105.38908000000001</v>
@@ -14241,7 +14241,7 @@
         <v>107.6</v>
       </c>
       <c r="J295" s="3">
-        <v>116.07</v>
+        <v>115.64059078492799</v>
       </c>
       <c r="K295" s="3">
         <v>104.14389</v>
@@ -14291,7 +14291,7 @@
         <v>107.4</v>
       </c>
       <c r="J296" s="3">
-        <v>117.02</v>
+        <v>116.48877674393199</v>
       </c>
       <c r="K296" s="3">
         <v>104.13106999999999</v>
@@ -14339,7 +14339,7 @@
         <v>104.3</v>
       </c>
       <c r="J297" s="3">
-        <v>117.16</v>
+        <v>117.09397123745499</v>
       </c>
       <c r="K297" s="3">
         <v>101.92055000000001</v>
@@ -14387,7 +14387,7 @@
         <v>107.2</v>
       </c>
       <c r="J298" s="3">
-        <v>117.87</v>
+        <v>117.755541107196</v>
       </c>
       <c r="K298" s="3">
         <v>101.33404</v>
@@ -14437,7 +14437,7 @@
         <v>109.2</v>
       </c>
       <c r="J299" s="3">
-        <v>119.27</v>
+        <v>118.989057773832</v>
       </c>
       <c r="K299" s="3">
         <v>102.25449999999999</v>
@@ -14485,7 +14485,7 @@
         <v>108.1</v>
       </c>
       <c r="J300" s="3">
-        <v>121.04</v>
+        <v>120.73437520739</v>
       </c>
       <c r="K300" s="3">
         <v>104.30741999999999</v>
@@ -14533,7 +14533,7 @@
         <v>108.6</v>
       </c>
       <c r="J301" s="3">
-        <v>120.96</v>
+        <v>121.32857747494801</v>
       </c>
       <c r="K301" s="3">
         <v>106.78988</v>
@@ -14583,7 +14583,7 @@
         <v>106.2</v>
       </c>
       <c r="J302" s="3">
-        <v>120.53</v>
+        <v>121.140077841562</v>
       </c>
       <c r="K302" s="3">
         <v>108.09201</v>
@@ -14631,7 +14631,7 @@
         <v>105.8</v>
       </c>
       <c r="J303" s="3">
-        <v>120.28</v>
+        <v>121.407756733935</v>
       </c>
       <c r="K303" s="3">
         <v>108.36733</v>
@@ -14679,7 +14679,7 @@
         <v>107.2</v>
       </c>
       <c r="J304" s="3">
-        <v>121.25</v>
+        <v>121.727968789342</v>
       </c>
       <c r="K304" s="3">
         <v>107.42533</v>
@@ -14729,7 +14729,7 @@
         <v>106.6</v>
       </c>
       <c r="J305" s="3">
-        <v>122.35</v>
+        <v>122.115046049429</v>
       </c>
       <c r="K305" s="3">
         <v>108.49863000000001</v>
@@ -14777,7 +14777,7 @@
         <v>103.2</v>
       </c>
       <c r="J306" s="3">
-        <v>123.13</v>
+        <v>122.505489657437</v>
       </c>
       <c r="K306" s="3">
         <v>110.74669</v>
@@ -14825,7 +14825,7 @@
         <v>106.9</v>
       </c>
       <c r="J307" s="3">
-        <v>123.17</v>
+        <v>122.692038827725</v>
       </c>
       <c r="K307" s="3">
         <v>110.22071</v>
@@ -14875,7 +14875,7 @@
         <v>105</v>
       </c>
       <c r="J308" s="3">
-        <v>123.48</v>
+        <v>122.90353645343301</v>
       </c>
       <c r="K308" s="3">
         <v>111.34265000000001</v>
@@ -14923,7 +14923,7 @@
         <v>103.1</v>
       </c>
       <c r="J309" s="3">
-        <v>123.37</v>
+        <v>123.241728574028</v>
       </c>
       <c r="K309" s="3">
         <v>113.27105</v>
@@ -14971,7 +14971,7 @@
         <v>105.2</v>
       </c>
       <c r="J310" s="3">
-        <v>124.04</v>
+        <v>123.788420067085</v>
       </c>
       <c r="K310" s="3">
         <v>112.59124</v>
@@ -15021,7 +15021,7 @@
         <v>103.7</v>
       </c>
       <c r="J311" s="3">
-        <v>124.44</v>
+        <v>124.136162999216</v>
       </c>
       <c r="K311" s="3">
         <v>111.95774</v>
@@ -15069,7 +15069,7 @@
         <v>103.4</v>
       </c>
       <c r="J312" s="3">
-        <v>124.55</v>
+        <v>124.36697183989899</v>
       </c>
       <c r="K312" s="3">
         <v>111.52255</v>
@@ -15117,7 +15117,7 @@
         <v>104</v>
       </c>
       <c r="J313" s="3">
-        <v>123.86</v>
+        <v>124.51459029573699</v>
       </c>
       <c r="K313" s="3">
         <v>111.87119</v>
@@ -15165,7 +15165,7 @@
       </c>
       <c r="I314" s="3"/>
       <c r="J314" s="3">
-        <v>124.06</v>
+        <v>124.920372802548</v>
       </c>
       <c r="K314" s="3">
         <v>110.7641</v>

</xml_diff>

<commit_message>
delete test data for models to check if they work, add ecb projections data and add chart
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\macrometrics-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973785C6-9407-4CD2-97EE-843B7628CCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820FDB31-A390-4C13-98D2-07CE07C976A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F32B473C-63B6-4416-A168-9B62820A9C8D}"/>
   </bookViews>
@@ -470,10 +470,10 @@
   <dimension ref="B2:Q315"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>